<commit_message>
update u2 stack and queue
</commit_message>
<xml_diff>
--- a/L2第2课栈和队列/队列和栈.xlsx
+++ b/L2第2课栈和队列/队列和栈.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XTL\2023_项目\L2第2课栈和队列\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XTL\2023_项目\L2_ebook\L2第2课栈和队列\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C324D59-CC65-446F-8162-563F4414E9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC3780B7-58CE-466A-8B70-347A655F8331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{CBEBB3EC-A2D4-4F71-B654-CE07A2B5B64B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{CBEBB3EC-A2D4-4F71-B654-CE07A2B5B64B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="stack" sheetId="1" r:id="rId1"/>
+    <sheet name="queue" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>栈</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,12 +93,69 @@
     <t>出栈 top--；</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>队列q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>↑</t>
+  </si>
+  <si>
+    <t>↑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tt是指向队尾的指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hh是指向队头的指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>↑↑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hh  tt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一步：右移队尾指针tt
+代码tt++;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二步：将元素x保存在tt位置 
+代码q[tt] = x;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>右移队头指针hh
+代码 hh++;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> tt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">hh </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +166,23 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -128,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -160,20 +235,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -182,10 +265,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -504,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6777B20F-B830-4F41-86B5-281601C6608C}">
   <dimension ref="B1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+    <sheetView topLeftCell="F3" workbookViewId="0">
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
@@ -617,8 +712,8 @@
     <row r="6" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -645,8 +740,8 @@
     <row r="7" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -667,21 +762,21 @@
     <row r="8" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="6" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="6" t="s">
+      <c r="O8" s="3"/>
+      <c r="P8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q8" s="1"/>
@@ -697,23 +792,23 @@
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="6" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="6" t="s">
+      <c r="O9" s="3"/>
+      <c r="P9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="Q9" s="1"/>
@@ -727,14 +822,14 @@
     <row r="10" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="1">
@@ -742,14 +837,14 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="6">
+      <c r="K10" s="3"/>
+      <c r="L10" s="4">
         <v>2</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="6">
+      <c r="O10" s="3"/>
+      <c r="P10" s="4">
         <v>2</v>
       </c>
       <c r="Q10" s="1"/>
@@ -763,12 +858,12 @@
     <row r="11" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H11" s="1">
@@ -778,18 +873,18 @@
       <c r="J11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="6">
+      <c r="K11" s="3"/>
+      <c r="L11" s="4">
         <v>1</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="4">
         <v>1</v>
       </c>
       <c r="Q11" s="1"/>
@@ -803,29 +898,29 @@
     <row r="12" spans="2:23" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="4">
         <v>0</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="4">
         <v>0</v>
       </c>
       <c r="Q12" s="1"/>
@@ -868,13 +963,13 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="6" t="s">
+      <c r="O14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="P14" s="1"/>
@@ -990,8 +1085,8 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="6" t="s">
+      <c r="O19" s="3"/>
+      <c r="P19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q19" s="1"/>
@@ -1013,8 +1108,8 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="6" t="s">
+      <c r="O20" s="3"/>
+      <c r="P20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="Q20" s="1"/>
@@ -1036,8 +1131,8 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="6">
+      <c r="O21" s="3"/>
+      <c r="P21" s="4">
         <v>2</v>
       </c>
       <c r="Q21" s="1"/>
@@ -1058,10 +1153,10 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P22" s="6">
+      <c r="P22" s="4">
         <v>1</v>
       </c>
       <c r="Q22" s="1"/>
@@ -1085,10 +1180,10 @@
       <c r="N23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P23" s="6">
+      <c r="P23" s="4">
         <v>0</v>
       </c>
       <c r="Q23" s="1"/>
@@ -1131,7 +1226,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="6" t="s">
+      <c r="O25" s="4" t="s">
         <v>7</v>
       </c>
       <c r="P25" s="1"/>
@@ -1360,4 +1455,3479 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FC1DF4-963A-4AA1-A8C9-86E6DE00DBE9}">
+  <dimension ref="A1:P192"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="88.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4">
+        <v>4</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>6</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" ht="71.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4</v>
+      </c>
+      <c r="H20" s="4">
+        <v>5</v>
+      </c>
+      <c r="I20" s="4">
+        <v>6</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" ht="31.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" ht="84.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4">
+        <v>-1</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2</v>
+      </c>
+      <c r="F26" s="4">
+        <v>3</v>
+      </c>
+      <c r="G26" s="4">
+        <v>4</v>
+      </c>
+      <c r="H26" s="4">
+        <v>5</v>
+      </c>
+      <c r="I26" s="4">
+        <v>6</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" ht="34.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
+      <c r="P107" s="1"/>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+      <c r="P109" s="1"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="1"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1"/>
+      <c r="P111" s="1"/>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+      <c r="P114" s="1"/>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+      <c r="O115" s="1"/>
+      <c r="P115" s="1"/>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+      <c r="N116" s="1"/>
+      <c r="O116" s="1"/>
+      <c r="P116" s="1"/>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+      <c r="O117" s="1"/>
+      <c r="P117" s="1"/>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+      <c r="O118" s="1"/>
+      <c r="P118" s="1"/>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+      <c r="N119" s="1"/>
+      <c r="O119" s="1"/>
+      <c r="P119" s="1"/>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+      <c r="N120" s="1"/>
+      <c r="O120" s="1"/>
+      <c r="P120" s="1"/>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="M121" s="1"/>
+      <c r="N121" s="1"/>
+      <c r="O121" s="1"/>
+      <c r="P121" s="1"/>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+      <c r="O122" s="1"/>
+      <c r="P122" s="1"/>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+      <c r="N123" s="1"/>
+      <c r="O123" s="1"/>
+      <c r="P123" s="1"/>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+      <c r="L124" s="1"/>
+      <c r="M124" s="1"/>
+      <c r="N124" s="1"/>
+      <c r="O124" s="1"/>
+      <c r="P124" s="1"/>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+      <c r="L125" s="1"/>
+      <c r="M125" s="1"/>
+      <c r="N125" s="1"/>
+      <c r="O125" s="1"/>
+      <c r="P125" s="1"/>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1"/>
+      <c r="P126" s="1"/>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+      <c r="L127" s="1"/>
+      <c r="M127" s="1"/>
+      <c r="N127" s="1"/>
+      <c r="O127" s="1"/>
+      <c r="P127" s="1"/>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+      <c r="L128" s="1"/>
+      <c r="M128" s="1"/>
+      <c r="N128" s="1"/>
+      <c r="O128" s="1"/>
+      <c r="P128" s="1"/>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="1"/>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+      <c r="L129" s="1"/>
+      <c r="M129" s="1"/>
+      <c r="N129" s="1"/>
+      <c r="O129" s="1"/>
+      <c r="P129" s="1"/>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+      <c r="L130" s="1"/>
+      <c r="M130" s="1"/>
+      <c r="N130" s="1"/>
+      <c r="O130" s="1"/>
+      <c r="P130" s="1"/>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="M131" s="1"/>
+      <c r="N131" s="1"/>
+      <c r="O131" s="1"/>
+      <c r="P131" s="1"/>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="P132" s="1"/>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+      <c r="O133" s="1"/>
+      <c r="P133" s="1"/>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="P134" s="1"/>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="M136" s="1"/>
+      <c r="N136" s="1"/>
+      <c r="O136" s="1"/>
+      <c r="P136" s="1"/>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="M137" s="1"/>
+      <c r="N137" s="1"/>
+      <c r="O137" s="1"/>
+      <c r="P137" s="1"/>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
+      <c r="O138" s="1"/>
+      <c r="P138" s="1"/>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="M139" s="1"/>
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="N140" s="1"/>
+      <c r="O140" s="1"/>
+      <c r="P140" s="1"/>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="M141" s="1"/>
+      <c r="N141" s="1"/>
+      <c r="O141" s="1"/>
+      <c r="P141" s="1"/>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1"/>
+      <c r="N142" s="1"/>
+      <c r="O142" s="1"/>
+      <c r="P142" s="1"/>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="M143" s="1"/>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1"/>
+      <c r="P143" s="1"/>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="M144" s="1"/>
+      <c r="N144" s="1"/>
+      <c r="O144" s="1"/>
+      <c r="P144" s="1"/>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="1"/>
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+      <c r="I145" s="1"/>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+      <c r="L145" s="1"/>
+      <c r="M145" s="1"/>
+      <c r="N145" s="1"/>
+      <c r="O145" s="1"/>
+      <c r="P145" s="1"/>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="M146" s="1"/>
+      <c r="N146" s="1"/>
+      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+      <c r="L147" s="1"/>
+      <c r="M147" s="1"/>
+      <c r="N147" s="1"/>
+      <c r="O147" s="1"/>
+      <c r="P147" s="1"/>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
+      <c r="J148" s="1"/>
+      <c r="K148" s="1"/>
+      <c r="L148" s="1"/>
+      <c r="M148" s="1"/>
+      <c r="N148" s="1"/>
+      <c r="O148" s="1"/>
+      <c r="P148" s="1"/>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+      <c r="I149" s="1"/>
+      <c r="J149" s="1"/>
+      <c r="K149" s="1"/>
+      <c r="L149" s="1"/>
+      <c r="M149" s="1"/>
+      <c r="N149" s="1"/>
+      <c r="O149" s="1"/>
+      <c r="P149" s="1"/>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
+      <c r="N150" s="1"/>
+      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="M152" s="1"/>
+      <c r="N152" s="1"/>
+      <c r="O152" s="1"/>
+      <c r="P152" s="1"/>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+      <c r="L153" s="1"/>
+      <c r="M153" s="1"/>
+      <c r="N153" s="1"/>
+      <c r="O153" s="1"/>
+      <c r="P153" s="1"/>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="M154" s="1"/>
+      <c r="N154" s="1"/>
+      <c r="O154" s="1"/>
+      <c r="P154" s="1"/>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="M155" s="1"/>
+      <c r="N155" s="1"/>
+      <c r="O155" s="1"/>
+      <c r="P155" s="1"/>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
+      <c r="O156" s="1"/>
+      <c r="P156" s="1"/>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="M157" s="1"/>
+      <c r="N157" s="1"/>
+      <c r="O157" s="1"/>
+      <c r="P157" s="1"/>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+      <c r="L158" s="1"/>
+      <c r="M158" s="1"/>
+      <c r="N158" s="1"/>
+      <c r="O158" s="1"/>
+      <c r="P158" s="1"/>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="1"/>
+      <c r="O159" s="1"/>
+      <c r="P159" s="1"/>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
+      <c r="O160" s="1"/>
+      <c r="P160" s="1"/>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="M161" s="1"/>
+      <c r="N161" s="1"/>
+      <c r="O161" s="1"/>
+      <c r="P161" s="1"/>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
+      <c r="I162" s="1"/>
+      <c r="J162" s="1"/>
+      <c r="K162" s="1"/>
+      <c r="L162" s="1"/>
+      <c r="M162" s="1"/>
+      <c r="N162" s="1"/>
+      <c r="O162" s="1"/>
+      <c r="P162" s="1"/>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+      <c r="H163" s="1"/>
+      <c r="I163" s="1"/>
+      <c r="J163" s="1"/>
+      <c r="K163" s="1"/>
+      <c r="L163" s="1"/>
+      <c r="M163" s="1"/>
+      <c r="N163" s="1"/>
+      <c r="O163" s="1"/>
+      <c r="P163" s="1"/>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+      <c r="H164" s="1"/>
+      <c r="I164" s="1"/>
+      <c r="J164" s="1"/>
+      <c r="K164" s="1"/>
+      <c r="L164" s="1"/>
+      <c r="M164" s="1"/>
+      <c r="N164" s="1"/>
+      <c r="O164" s="1"/>
+      <c r="P164" s="1"/>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="1"/>
+      <c r="H165" s="1"/>
+      <c r="I165" s="1"/>
+      <c r="J165" s="1"/>
+      <c r="K165" s="1"/>
+      <c r="L165" s="1"/>
+      <c r="M165" s="1"/>
+      <c r="N165" s="1"/>
+      <c r="O165" s="1"/>
+      <c r="P165" s="1"/>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+      <c r="H166" s="1"/>
+      <c r="I166" s="1"/>
+      <c r="J166" s="1"/>
+      <c r="K166" s="1"/>
+      <c r="L166" s="1"/>
+      <c r="M166" s="1"/>
+      <c r="N166" s="1"/>
+      <c r="O166" s="1"/>
+      <c r="P166" s="1"/>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1"/>
+      <c r="I167" s="1"/>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
+      <c r="L167" s="1"/>
+      <c r="M167" s="1"/>
+      <c r="N167" s="1"/>
+      <c r="O167" s="1"/>
+      <c r="P167" s="1"/>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+      <c r="I168" s="1"/>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+      <c r="L168" s="1"/>
+      <c r="M168" s="1"/>
+      <c r="N168" s="1"/>
+      <c r="O168" s="1"/>
+      <c r="P168" s="1"/>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+      <c r="I169" s="1"/>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="1"/>
+      <c r="N169" s="1"/>
+      <c r="O169" s="1"/>
+      <c r="P169" s="1"/>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+      <c r="I170" s="1"/>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+      <c r="L170" s="1"/>
+      <c r="M170" s="1"/>
+      <c r="N170" s="1"/>
+      <c r="O170" s="1"/>
+      <c r="P170" s="1"/>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+      <c r="I171" s="1"/>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+      <c r="L171" s="1"/>
+      <c r="M171" s="1"/>
+      <c r="N171" s="1"/>
+      <c r="O171" s="1"/>
+      <c r="P171" s="1"/>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
+      <c r="I172" s="1"/>
+      <c r="J172" s="1"/>
+      <c r="K172" s="1"/>
+      <c r="L172" s="1"/>
+      <c r="M172" s="1"/>
+      <c r="N172" s="1"/>
+      <c r="O172" s="1"/>
+      <c r="P172" s="1"/>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
+      <c r="H173" s="1"/>
+      <c r="I173" s="1"/>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+      <c r="L173" s="1"/>
+      <c r="M173" s="1"/>
+      <c r="N173" s="1"/>
+      <c r="O173" s="1"/>
+      <c r="P173" s="1"/>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+      <c r="H174" s="1"/>
+      <c r="I174" s="1"/>
+      <c r="J174" s="1"/>
+      <c r="K174" s="1"/>
+      <c r="L174" s="1"/>
+      <c r="M174" s="1"/>
+      <c r="N174" s="1"/>
+      <c r="O174" s="1"/>
+      <c r="P174" s="1"/>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+      <c r="H175" s="1"/>
+      <c r="I175" s="1"/>
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+      <c r="L175" s="1"/>
+      <c r="M175" s="1"/>
+      <c r="N175" s="1"/>
+      <c r="O175" s="1"/>
+      <c r="P175" s="1"/>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+      <c r="G176" s="1"/>
+      <c r="H176" s="1"/>
+      <c r="I176" s="1"/>
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+      <c r="L176" s="1"/>
+      <c r="M176" s="1"/>
+      <c r="N176" s="1"/>
+      <c r="O176" s="1"/>
+      <c r="P176" s="1"/>
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="1"/>
+      <c r="G177" s="1"/>
+      <c r="H177" s="1"/>
+      <c r="I177" s="1"/>
+      <c r="J177" s="1"/>
+      <c r="K177" s="1"/>
+      <c r="L177" s="1"/>
+      <c r="M177" s="1"/>
+      <c r="N177" s="1"/>
+      <c r="O177" s="1"/>
+      <c r="P177" s="1"/>
+    </row>
+    <row r="178" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="1"/>
+      <c r="H178" s="1"/>
+      <c r="I178" s="1"/>
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+      <c r="L178" s="1"/>
+      <c r="M178" s="1"/>
+      <c r="N178" s="1"/>
+      <c r="O178" s="1"/>
+      <c r="P178" s="1"/>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="1"/>
+      <c r="H179" s="1"/>
+      <c r="I179" s="1"/>
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+      <c r="L179" s="1"/>
+      <c r="M179" s="1"/>
+      <c r="N179" s="1"/>
+      <c r="O179" s="1"/>
+      <c r="P179" s="1"/>
+    </row>
+    <row r="180" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="1"/>
+      <c r="H180" s="1"/>
+      <c r="I180" s="1"/>
+      <c r="J180" s="1"/>
+      <c r="K180" s="1"/>
+      <c r="L180" s="1"/>
+      <c r="M180" s="1"/>
+      <c r="N180" s="1"/>
+      <c r="O180" s="1"/>
+      <c r="P180" s="1"/>
+    </row>
+    <row r="181" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="1"/>
+      <c r="H181" s="1"/>
+      <c r="I181" s="1"/>
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+      <c r="L181" s="1"/>
+      <c r="M181" s="1"/>
+      <c r="N181" s="1"/>
+      <c r="O181" s="1"/>
+      <c r="P181" s="1"/>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="1"/>
+      <c r="F182" s="1"/>
+      <c r="G182" s="1"/>
+      <c r="H182" s="1"/>
+      <c r="I182" s="1"/>
+      <c r="J182" s="1"/>
+      <c r="K182" s="1"/>
+      <c r="L182" s="1"/>
+      <c r="M182" s="1"/>
+      <c r="N182" s="1"/>
+      <c r="O182" s="1"/>
+      <c r="P182" s="1"/>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="1"/>
+      <c r="G183" s="1"/>
+      <c r="H183" s="1"/>
+      <c r="I183" s="1"/>
+      <c r="J183" s="1"/>
+      <c r="K183" s="1"/>
+      <c r="L183" s="1"/>
+      <c r="M183" s="1"/>
+      <c r="N183" s="1"/>
+      <c r="O183" s="1"/>
+      <c r="P183" s="1"/>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1"/>
+      <c r="E184" s="1"/>
+      <c r="F184" s="1"/>
+      <c r="G184" s="1"/>
+      <c r="H184" s="1"/>
+      <c r="I184" s="1"/>
+      <c r="J184" s="1"/>
+      <c r="K184" s="1"/>
+      <c r="L184" s="1"/>
+      <c r="M184" s="1"/>
+      <c r="N184" s="1"/>
+      <c r="O184" s="1"/>
+      <c r="P184" s="1"/>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1"/>
+      <c r="E185" s="1"/>
+      <c r="F185" s="1"/>
+      <c r="G185" s="1"/>
+      <c r="H185" s="1"/>
+      <c r="I185" s="1"/>
+      <c r="J185" s="1"/>
+      <c r="K185" s="1"/>
+      <c r="L185" s="1"/>
+      <c r="M185" s="1"/>
+      <c r="N185" s="1"/>
+      <c r="O185" s="1"/>
+      <c r="P185" s="1"/>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
+      <c r="G186" s="1"/>
+      <c r="H186" s="1"/>
+      <c r="I186" s="1"/>
+      <c r="J186" s="1"/>
+      <c r="K186" s="1"/>
+      <c r="L186" s="1"/>
+      <c r="M186" s="1"/>
+      <c r="N186" s="1"/>
+      <c r="O186" s="1"/>
+      <c r="P186" s="1"/>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="1"/>
+      <c r="D187" s="1"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="M187" s="1"/>
+      <c r="N187" s="1"/>
+      <c r="O187" s="1"/>
+      <c r="P187" s="1"/>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
+      <c r="C188" s="1"/>
+      <c r="D188" s="1"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
+      <c r="G188" s="1"/>
+      <c r="H188" s="1"/>
+      <c r="I188" s="1"/>
+      <c r="J188" s="1"/>
+      <c r="K188" s="1"/>
+      <c r="L188" s="1"/>
+      <c r="M188" s="1"/>
+      <c r="N188" s="1"/>
+      <c r="O188" s="1"/>
+      <c r="P188" s="1"/>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
+      <c r="C189" s="1"/>
+      <c r="D189" s="1"/>
+      <c r="E189" s="1"/>
+      <c r="F189" s="1"/>
+      <c r="G189" s="1"/>
+      <c r="H189" s="1"/>
+      <c r="I189" s="1"/>
+      <c r="J189" s="1"/>
+      <c r="K189" s="1"/>
+      <c r="L189" s="1"/>
+      <c r="M189" s="1"/>
+      <c r="N189" s="1"/>
+      <c r="O189" s="1"/>
+      <c r="P189" s="1"/>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="1"/>
+      <c r="E190" s="1"/>
+      <c r="F190" s="1"/>
+      <c r="G190" s="1"/>
+      <c r="H190" s="1"/>
+      <c r="I190" s="1"/>
+      <c r="J190" s="1"/>
+      <c r="K190" s="1"/>
+      <c r="L190" s="1"/>
+      <c r="M190" s="1"/>
+      <c r="N190" s="1"/>
+      <c r="O190" s="1"/>
+      <c r="P190" s="1"/>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
+      <c r="C191" s="1"/>
+      <c r="D191" s="1"/>
+      <c r="E191" s="1"/>
+      <c r="F191" s="1"/>
+      <c r="G191" s="1"/>
+      <c r="H191" s="1"/>
+      <c r="I191" s="1"/>
+      <c r="J191" s="1"/>
+      <c r="K191" s="1"/>
+      <c r="L191" s="1"/>
+      <c r="M191" s="1"/>
+      <c r="N191" s="1"/>
+      <c r="O191" s="1"/>
+      <c r="P191" s="1"/>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+      <c r="D192" s="1"/>
+      <c r="E192" s="1"/>
+      <c r="F192" s="1"/>
+      <c r="G192" s="1"/>
+      <c r="H192" s="1"/>
+      <c r="I192" s="1"/>
+      <c r="J192" s="1"/>
+      <c r="K192" s="1"/>
+      <c r="L192" s="1"/>
+      <c r="M192" s="1"/>
+      <c r="N192" s="1"/>
+      <c r="O192" s="1"/>
+      <c r="P192" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B29:I29"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>